<commit_message>
Hawaii 2010 NHPI our_approach table - pop data edit
</commit_message>
<xml_diff>
--- a/AAJC Vis/case_studies/our_approach_tables.xlsx
+++ b/AAJC Vis/case_studies/our_approach_tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anamkhan/Documents/Demo Advisors/AAJC/AAJC Vis/case_studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACAA50E-FCC5-7143-AC20-EDD862C2710B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD4C9DD9-AC6A-0F45-9017-E77CA28FA1E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17220" activeTab="6" xr2:uid="{C07E5E56-DC6A-294B-AF7A-B661110C6B4A}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17180" activeTab="4" xr2:uid="{C07E5E56-DC6A-294B-AF7A-B661110C6B4A}"/>
   </bookViews>
   <sheets>
     <sheet name="LA - CA" sheetId="1" r:id="rId1"/>
@@ -2677,8 +2677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36E1BC0B-CFFE-6E45-9286-B114DD216D97}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="117" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2994,12 +2994,12 @@
         <v>36188</v>
       </c>
       <c r="M11" s="9">
-        <f>SUM(M6:M10)</f>
-        <v>1395468</v>
+        <f>C11+E11+G11+I11+K11</f>
+        <v>120469</v>
       </c>
       <c r="N11" s="10">
-        <f>SUM(N6:N10)</f>
-        <v>1757075</v>
+        <f>D11+F11+H11+J11+L11</f>
+        <v>289888</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
@@ -3037,12 +3037,12 @@
         <v>42734</v>
       </c>
       <c r="M12" s="11">
-        <f>SUM(M7:M11)</f>
-        <v>2790936</v>
+        <f>C12+E12+G12+I12+K12</f>
+        <v>138292</v>
       </c>
       <c r="N12" s="10">
-        <f>SUM(N7:N11)</f>
-        <v>3514150</v>
+        <f>D12+F12+H12+J12+L12</f>
+        <v>358951</v>
       </c>
     </row>
     <row r="13" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -4408,7 +4408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C7E884C-2B29-8846-B987-863484516567}">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>

</xml_diff>